<commit_message>
Enabled the review process to write to the reviews file
</commit_message>
<xml_diff>
--- a/tests/data/Test_User_Reviews.xlsx
+++ b/tests/data/Test_User_Reviews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,125 +434,154 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>UID</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Scholarship</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>UID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Scholarship</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Additional Feedback</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="A2" t="n">
+        <v>1500643</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cool Kids</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1577306</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cool Kids</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1522661</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cool Kids</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>1582872</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Test One</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>This student would be a good pick for Test One</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cool Kids</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>1536237</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Test One</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Cool Kids</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
+    <row r="7">
+      <c r="A7" t="n">
         <v>1500178</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>Test One</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Cool Kids</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>The Club</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>1536237</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Cool Kids</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>The Club</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>1500178</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Cool Kids</t>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>The Club</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added selection clearing after review
</commit_message>
<xml_diff>
--- a/tests/data/Test_User_Reviews.xlsx
+++ b/tests/data/Test_User_Reviews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +585,747 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Hey there kiddo</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Hey there kiddo</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Hey there kiddo</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>One more time</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>One more time</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>One more time</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1500643</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>heyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1577306</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>heyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1522661</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>heyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1500643</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>yu[</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1577306</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>yu[</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1522661</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>yu[</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1555608</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1564859</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1519712</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1565818</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1564859</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1519712</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1564859</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1519712</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1519712</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1519712</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Testing this for real</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Testing this for real</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Testing this for real</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>1500643</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Testing this for real</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ok Ok </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ok Ok </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1500178</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ok Ok </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a success feedback to recommendation form
</commit_message>
<xml_diff>
--- a/tests/data/Test_User_Reviews.xlsx
+++ b/tests/data/Test_User_Reviews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1326,6 +1326,81 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1582872</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1536237</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Yup</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1519712</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Oh yeah</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1565818</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Oh yeah</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>1506281</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Oh yeah</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fix for state saving
</commit_message>
<xml_diff>
--- a/tests/data/Test_User_Reviews.xlsx
+++ b/tests/data/Test_User_Reviews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,78 +452,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1578155</v>
+        <v>1582872</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Test One</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yup</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1592827</v>
+        <v>1582872</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Yup</t>
-        </is>
-      </c>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1512179</v>
+        <v>1536237</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Yup</t>
-        </is>
-      </c>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1582872</v>
+        <v>1500178</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Hey</t>
-        </is>
-      </c>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1536237</v>
+        <v>1500643</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Hey</t>
-        </is>
-      </c>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -534,26 +514,29 @@
           <t>Test One</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Hey</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1518928</v>
+        <v>1500643</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Test One</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>These guys look good</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1577306</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Needed to change linitng to allow me to use a global variable
</commit_message>
<xml_diff>
--- a/tests/data/Test_User_Reviews.xlsx
+++ b/tests/data/Test_User_Reviews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,6 +538,21 @@
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1536869</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test One</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>These guys are good</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added yes no maybe ability to recommendations
</commit_message>
<xml_diff>
--- a/tests/data/Test_User_Reviews.xlsx
+++ b/tests/data/Test_User_Reviews.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Rating</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Additional Feedback</t>
         </is>
       </c>
@@ -459,97 +464,14 @@
           <t>Test One</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1582872</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Cool Kids Club</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1536237</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Cool Kids Club</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1500178</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cool Kids Club</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1500643</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cool Kids Club</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1500178</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1500643</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1577306</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1536869</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Test One</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>These guys are good</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Maybe</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Idk about this person</t>
         </is>
       </c>
     </row>

</xml_diff>